<commit_message>
Ready to be released
Changed progress bar; updated screen outputs
</commit_message>
<xml_diff>
--- a/results/stars_with_bright_neighbors.xlsx
+++ b/results/stars_with_bright_neighbors.xlsx
@@ -998,7 +998,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1462061709996744448</t>
+          <t>1462061709995883136</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1462061709995883136</t>
+          <t>1462061709996744448</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3894474759723667200</t>
+          <t>3894474755427985408</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3894474755427985408</t>
+          <t>3894474759723667200</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4207995002827396224</t>
+          <t>4207995002838460800</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4207995002838460800</t>
+          <t>4207995002827396224</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4316214125609944832</t>
+          <t>4316214125587568896</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4316214125587568896</t>
+          <t>4316214125609944832</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3213958769589070848</t>
+          <t>3213958769587525888</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3213958769587525888</t>
+          <t>3213958769589070848</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3420,7 +3420,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3514475535345385728</t>
+          <t>3514475531051071488</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3514475531051071488</t>
+          <t>3514475535345385728</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6529537521961887360</t>
+          <t>6529537526254976768</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6529537526254976768</t>
+          <t>6529537521961887360</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1837182676173127680</t>
+          <t>1837182676179555712</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1837182676179555712</t>
+          <t>1837182676173127680</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4692276170590701952</t>
+          <t>4692276170589724288</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -4931,7 +4931,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4692276170589724288</t>
+          <t>4692276170590701952</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5200,7 +5200,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>3054910392543754752</t>
+          <t>3054910392548138752</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -5283,7 +5283,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>3054910392548138752</t>
+          <t>3054910392543754752</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="Y58" t="inlineStr">
         <is>
-          <t>HighPM*</t>
+          <t>SB*</t>
         </is>
       </c>
       <c r="Z58" t="inlineStr">
@@ -5855,7 +5855,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>3511580658668406528</t>
+          <t>3511580654376012928</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>3511580654376012928</t>
+          <t>3511580658668406528</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -6278,282 +6278,282 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>4187404036259094528</t>
+          <t>6298476051032199936</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4187404036259094528</t>
+          <t>6298476051032199936</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>4187404036259094528</t>
+          <t>6298476051032199936</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>292.0512585965648</v>
+        <v>217.8337361899387</v>
       </c>
       <c r="E68" t="n">
-        <v>-12.145184777159</v>
+        <v>-15.64037537479623</v>
       </c>
       <c r="F68" t="n">
-        <v>8.213438034057617</v>
+        <v>8.668020908975601</v>
       </c>
       <c r="G68" t="n">
-        <v>8.213438034057617</v>
+        <v>9.035721778869629</v>
       </c>
       <c r="H68" t="n">
-        <v>7.808540344238281</v>
+        <v>8.90089225769043</v>
       </c>
       <c r="I68" t="n">
-        <v>6.908134937286377</v>
+        <v>7.66861629486084</v>
       </c>
       <c r="J68" t="n">
-        <v>0.9004054069519043</v>
+        <v>1.23227596282959</v>
       </c>
       <c r="K68" t="n">
-        <v>26.82442894269294</v>
+        <v>22.44221926782221</v>
       </c>
       <c r="L68" t="n">
         <v>5420.00849935214</v>
       </c>
       <c r="N68" t="n">
-        <v>1.169499555379738</v>
+        <v>1.056817527779121</v>
       </c>
       <c r="P68" t="n">
-        <v>1.496345366643906</v>
+        <v>1.422432991037836</v>
       </c>
       <c r="Q68" t="n">
-        <v>0.3120357937932556</v>
+        <v>0.3846989403186152</v>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>HD 183063B</t>
+          <t>HD 127356B</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>GJ 3854 B</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
           <t>HighPM*</t>
+        </is>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>K3?</t>
+        </is>
+      </c>
+      <c r="AB68" t="inlineStr">
+        <is>
+          <t>K3</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6298476051032199936</t>
+          <t>4187404036259094528</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6298476252895259520</t>
+          <t>4187404036259094528</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>6298476051032199936</t>
+          <t>4187404036259094528</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>217.8337361899387</v>
+        <v>292.0512585965648</v>
       </c>
       <c r="E69" t="n">
-        <v>-15.64037537479623</v>
+        <v>-12.145184777159</v>
       </c>
       <c r="F69" t="n">
-        <v>8.668020908975601</v>
+        <v>8.213438034057617</v>
       </c>
       <c r="G69" t="n">
-        <v>9.035721778869629</v>
+        <v>8.213438034057617</v>
       </c>
       <c r="H69" t="n">
-        <v>8.90089225769043</v>
+        <v>7.808540344238281</v>
       </c>
       <c r="I69" t="n">
-        <v>7.66861629486084</v>
+        <v>6.908134937286377</v>
       </c>
       <c r="J69" t="n">
-        <v>1.23227596282959</v>
+        <v>0.9004054069519043</v>
       </c>
       <c r="K69" t="n">
-        <v>22.44221926782221</v>
+        <v>26.82442894269294</v>
       </c>
       <c r="L69" t="n">
         <v>5420.00849935214</v>
       </c>
       <c r="N69" t="n">
-        <v>1.056817527779121</v>
+        <v>1.169499555379738</v>
       </c>
       <c r="P69" t="n">
-        <v>1.422432991037836</v>
+        <v>1.496345366643906</v>
       </c>
       <c r="Q69" t="n">
-        <v>0.3846989403186152</v>
+        <v>0.3120357937932556</v>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>HD 127356B</t>
-        </is>
-      </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>GJ 3854 B</t>
+          <t>HD 183063B</t>
         </is>
       </c>
       <c r="Y69" t="inlineStr">
         <is>
           <t>HighPM*</t>
-        </is>
-      </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>K3?</t>
-        </is>
-      </c>
-      <c r="AB69" t="inlineStr">
-        <is>
-          <t>K3</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>4187404036259094528</t>
+          <t>6298476051032199936</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>4187404036266621952</t>
+          <t>6298476252895259520</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>4187404036259094528</t>
+          <t>6298476051032199936</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>292.0512585965648</v>
+        <v>217.8337361899387</v>
       </c>
       <c r="E70" t="n">
-        <v>-12.145184777159</v>
+        <v>-15.64037537479623</v>
       </c>
       <c r="F70" t="n">
-        <v>8.213438034057617</v>
+        <v>8.668020908975601</v>
       </c>
       <c r="G70" t="n">
-        <v>8.213438034057617</v>
+        <v>9.035721778869629</v>
       </c>
       <c r="H70" t="n">
-        <v>7.808540344238281</v>
+        <v>8.90089225769043</v>
       </c>
       <c r="I70" t="n">
-        <v>6.908134937286377</v>
+        <v>7.66861629486084</v>
       </c>
       <c r="J70" t="n">
-        <v>0.9004054069519043</v>
+        <v>1.23227596282959</v>
       </c>
       <c r="K70" t="n">
-        <v>26.82442894269294</v>
+        <v>22.44221926782221</v>
       </c>
       <c r="L70" t="n">
         <v>5420.00849935214</v>
       </c>
       <c r="N70" t="n">
-        <v>1.169499555379738</v>
+        <v>1.056817527779121</v>
       </c>
       <c r="P70" t="n">
-        <v>1.496345366643906</v>
+        <v>1.422432991037836</v>
       </c>
       <c r="Q70" t="n">
-        <v>0.3120357937932556</v>
+        <v>0.3846989403186152</v>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>HD 183063B</t>
+          <t>HD 127356B</t>
+        </is>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>GJ 3854 B</t>
         </is>
       </c>
       <c r="Y70" t="inlineStr">
         <is>
           <t>HighPM*</t>
+        </is>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>K3?</t>
+        </is>
+      </c>
+      <c r="AB70" t="inlineStr">
+        <is>
+          <t>K3</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6298476051032199936</t>
+          <t>4187404036259094528</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6298476051032199936</t>
+          <t>4187404036266621952</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>6298476051032199936</t>
+          <t>4187404036259094528</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>217.8337361899387</v>
+        <v>292.0512585965648</v>
       </c>
       <c r="E71" t="n">
-        <v>-15.64037537479623</v>
+        <v>-12.145184777159</v>
       </c>
       <c r="F71" t="n">
-        <v>8.668020908975601</v>
+        <v>8.213438034057617</v>
       </c>
       <c r="G71" t="n">
-        <v>9.035721778869629</v>
+        <v>8.213438034057617</v>
       </c>
       <c r="H71" t="n">
-        <v>8.90089225769043</v>
+        <v>7.808540344238281</v>
       </c>
       <c r="I71" t="n">
-        <v>7.66861629486084</v>
+        <v>6.908134937286377</v>
       </c>
       <c r="J71" t="n">
-        <v>1.23227596282959</v>
+        <v>0.9004054069519043</v>
       </c>
       <c r="K71" t="n">
-        <v>22.44221926782221</v>
+        <v>26.82442894269294</v>
       </c>
       <c r="L71" t="n">
         <v>5420.00849935214</v>
       </c>
       <c r="N71" t="n">
-        <v>1.056817527779121</v>
+        <v>1.169499555379738</v>
       </c>
       <c r="P71" t="n">
-        <v>1.422432991037836</v>
+        <v>1.496345366643906</v>
       </c>
       <c r="Q71" t="n">
-        <v>0.3846989403186152</v>
+        <v>0.3120357937932556</v>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>HD 127356B</t>
-        </is>
-      </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>GJ 3854 B</t>
+          <t>HD 183063B</t>
         </is>
       </c>
       <c r="Y71" t="inlineStr">
         <is>
           <t>HighPM*</t>
-        </is>
-      </c>
-      <c r="AA71" t="inlineStr">
-        <is>
-          <t>K3?</t>
-        </is>
-      </c>
-      <c r="AB71" t="inlineStr">
-        <is>
-          <t>K3</t>
         </is>
       </c>
     </row>
@@ -6831,7 +6831,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>6700048793058633728</t>
+          <t>6700048793060566272</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6700048793060566272</t>
+          <t>6700048793058633728</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -7615,7 +7615,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>3312536923393893120</t>
+          <t>3312536927686011520</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -7630,19 +7630,19 @@
         <v>15.6381385358323</v>
       </c>
       <c r="F85" t="n">
-        <v>7.672853330383301</v>
+        <v>7.944008827209473</v>
       </c>
       <c r="G85" t="n">
         <v>7.944008827209473</v>
       </c>
       <c r="H85" t="n">
-        <v>7.905549049377441</v>
+        <v>5.725773334503174</v>
       </c>
       <c r="I85" t="n">
-        <v>6.680329322814941</v>
+        <v>5.313418865203857</v>
       </c>
       <c r="J85" t="n">
-        <v>1.2252197265625</v>
+        <v>0.4123544692993164</v>
       </c>
       <c r="K85" t="n">
         <v>21.33769931920589</v>
@@ -7663,10 +7663,10 @@
         <v>1.365843868772226</v>
       </c>
       <c r="Q85" t="n">
-        <v>0.2839703666371027</v>
+        <v>0.3217393066198116</v>
       </c>
       <c r="R85" t="n">
-        <v>3.711777761890294</v>
+        <v>4.205458838412122</v>
       </c>
       <c r="S85" t="n">
         <v>0.9648470258968647</v>
@@ -7700,7 +7700,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3312536927686011520</t>
+          <t>3312536923393893120</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -7715,19 +7715,19 @@
         <v>15.6381385358323</v>
       </c>
       <c r="F86" t="n">
-        <v>7.944008827209473</v>
+        <v>7.672853330383301</v>
       </c>
       <c r="G86" t="n">
         <v>7.944008827209473</v>
       </c>
       <c r="H86" t="n">
-        <v>5.725773334503174</v>
+        <v>7.905549049377441</v>
       </c>
       <c r="I86" t="n">
-        <v>5.313418865203857</v>
+        <v>6.680329322814941</v>
       </c>
       <c r="J86" t="n">
-        <v>0.4123544692993164</v>
+        <v>1.2252197265625</v>
       </c>
       <c r="K86" t="n">
         <v>21.33769931920589</v>
@@ -7748,10 +7748,10 @@
         <v>1.365843868772226</v>
       </c>
       <c r="Q86" t="n">
-        <v>0.3217393066198116</v>
+        <v>0.2839703666371027</v>
       </c>
       <c r="R86" t="n">
-        <v>4.205458838412122</v>
+        <v>3.711777761890294</v>
       </c>
       <c r="S86" t="n">
         <v>0.9648470258968647</v>
@@ -8039,7 +8039,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>4858250264007576320</t>
+          <t>4858250268302005760</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -8122,7 +8122,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>4858250268302005760</t>
+          <t>4858250264007576320</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -8205,7 +8205,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2739059700184753280</t>
+          <t>2739059700183271424</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -8226,13 +8226,7 @@
         <v>8.972273826599121</v>
       </c>
       <c r="H92" t="n">
-        <v>7.462995529174805</v>
-      </c>
-      <c r="I92" t="n">
-        <v>6.632507801055908</v>
-      </c>
-      <c r="J92" t="n">
-        <v>0.8304877281188965</v>
+        <v>7.701591491699219</v>
       </c>
       <c r="K92" t="n">
         <v>23.30923025364912</v>
@@ -8268,7 +8262,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2739059700183271424</t>
+          <t>2739059700184753280</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -8289,7 +8283,13 @@
         <v>8.972273826599121</v>
       </c>
       <c r="H93" t="n">
-        <v>7.701591491699219</v>
+        <v>7.462995529174805</v>
+      </c>
+      <c r="I93" t="n">
+        <v>6.632507801055908</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.8304877281188965</v>
       </c>
       <c r="K93" t="n">
         <v>23.30923025364912</v>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>5848710168188419456</t>
+          <t>5848710168215059584</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -8652,7 +8652,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>5848710168215059584</t>
+          <t>5848710168188419456</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -8715,131 +8715,131 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2019550767153854080</t>
+          <t>5650153795716877568</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2019550767177606016</t>
+          <t>5650153825784353280</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2019550767153854080</t>
+          <t>5650153795716877568</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>293.3591550413757</v>
+        <v>137.1509137769664</v>
       </c>
       <c r="E99" t="n">
-        <v>23.49786033326636</v>
+        <v>-25.83897499617422</v>
       </c>
       <c r="F99" t="n">
-        <v>11.95027923583984</v>
+        <v>11.61914443969727</v>
       </c>
       <c r="G99" t="n">
-        <v>11.95027923583984</v>
+        <v>11.61914443969727</v>
       </c>
       <c r="H99" t="n">
-        <v>7.998145580291748</v>
+        <v>6.943893432617188</v>
       </c>
       <c r="I99" t="n">
-        <v>7.178745269775391</v>
+        <v>6.195503234863281</v>
       </c>
       <c r="J99" t="n">
-        <v>0.8194003105163574</v>
+        <v>0.7483901977539062</v>
       </c>
       <c r="K99" t="n">
-        <v>21.33710135631854</v>
+        <v>22.40026209270729</v>
       </c>
       <c r="L99" t="n">
         <v>5956.622743314438</v>
       </c>
       <c r="N99" t="n">
-        <v>1.419057770979633</v>
+        <v>3.311311302082258</v>
       </c>
       <c r="P99" t="n">
-        <v>1.588051481584071</v>
+        <v>2.425853360885495</v>
       </c>
       <c r="Q99" t="n">
-        <v>2.189283159065488</v>
+        <v>1.879641292066385</v>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>HD 184403B</t>
+          <t>HD  78643B</t>
+        </is>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>GJ 9287 B</t>
         </is>
       </c>
       <c r="Y99" t="inlineStr">
         <is>
-          <t>Star</t>
+          <t>**</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>5650153795716877568</t>
+          <t>2019550767153854080</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>5650153825784353280</t>
+          <t>2019550767177606016</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>5650153795716877568</t>
+          <t>2019550767153854080</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>137.1509137769664</v>
+        <v>293.3591550413757</v>
       </c>
       <c r="E100" t="n">
-        <v>-25.83897499617422</v>
+        <v>23.49786033326636</v>
       </c>
       <c r="F100" t="n">
-        <v>11.61914443969727</v>
+        <v>11.95027923583984</v>
       </c>
       <c r="G100" t="n">
-        <v>11.61914443969727</v>
+        <v>11.95027923583984</v>
       </c>
       <c r="H100" t="n">
-        <v>6.943893432617188</v>
+        <v>7.998145580291748</v>
       </c>
       <c r="I100" t="n">
-        <v>6.195503234863281</v>
+        <v>7.178745269775391</v>
       </c>
       <c r="J100" t="n">
-        <v>0.7483901977539062</v>
+        <v>0.8194003105163574</v>
       </c>
       <c r="K100" t="n">
-        <v>22.40026209270729</v>
+        <v>21.33710135631854</v>
       </c>
       <c r="L100" t="n">
         <v>5956.622743314438</v>
       </c>
       <c r="N100" t="n">
-        <v>3.311311302082258</v>
+        <v>1.419057770979633</v>
       </c>
       <c r="P100" t="n">
-        <v>2.425853360885495</v>
+        <v>1.588051481584071</v>
       </c>
       <c r="Q100" t="n">
-        <v>1.879641292066385</v>
+        <v>2.189283159065488</v>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>HD  78643B</t>
-        </is>
-      </c>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>GJ 9287 B</t>
+          <t>HD 184403B</t>
         </is>
       </c>
       <c r="Y100" t="inlineStr">
         <is>
-          <t>**</t>
+          <t>Star</t>
         </is>
       </c>
     </row>
@@ -8977,7 +8977,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>1271209611223823232</t>
+          <t>1271209615518148736</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -9060,7 +9060,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>1271209615518148736</t>
+          <t>1271209611223823232</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">

</xml_diff>